<commit_message>
[FIX] category and grade removed
</commit_message>
<xml_diff>
--- a/public/format/Questions.xlsx
+++ b/public/format/Questions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mangosoft\Asmita Publication\storage\app\public\format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mangosoft\Asmita Publication\public\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,23 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Question</t>
   </si>
   <si>
-    <t>Question Type</t>
-  </si>
-  <si>
     <t>Marks</t>
   </si>
   <si>
-    <t>Option 1</t>
-  </si>
-  <si>
-    <t>Option 2</t>
-  </si>
-  <si>
     <t>Option 3</t>
   </si>
   <si>
@@ -51,13 +42,65 @@
   </si>
   <si>
     <t>Question Hint</t>
+  </si>
+  <si>
+    <t>Question Type (maq or mcq)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Option 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Option 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>What is 2 * 2?</t>
+  </si>
+  <si>
+    <t>mcq</t>
+  </si>
+  <si>
+    <t>maq</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>Which of them are prime numbers?</t>
+  </si>
+  <si>
+    <t>Please remove this message and 
+above demo question before adding question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +124,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -112,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -120,6 +170,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -402,23 +455,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
+    <col min="1" max="1" width="44" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="22.875" customWidth="1"/>
-    <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="25.875" customWidth="1"/>
-    <col min="6" max="6" width="34.375" customWidth="1"/>
-    <col min="7" max="7" width="22.875" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
+    <col min="6" max="6" width="13.75" customWidth="1"/>
+    <col min="7" max="7" width="15.25" customWidth="1"/>
     <col min="8" max="8" width="26.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" customWidth="1"/>
+    <col min="9" max="9" width="30.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -426,28 +479,85 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="G2">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
         <v>8</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>